<commit_message>
added ex 3, 7-10
</commit_message>
<xml_diff>
--- a/7/chi-squared_test_and_pearson_correlation.xlsx
+++ b/7/chi-squared_test_and_pearson_correlation.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="U:\Lektionen\DA_HS2022\KK\Week_07\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Data Analytics\7\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F11B7A82-03C4-4618-8318-8FB25E4CF166}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32F3E3B5-4F55-4189-8ADA-10E393FC9282}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-3924" yWindow="-17388" windowWidth="30936" windowHeight="16896" xr2:uid="{5EEC2E2C-3288-4F5E-82D1-2929FCEC1714}"/>
+    <workbookView xWindow="6490" yWindow="2470" windowWidth="19200" windowHeight="9970" xr2:uid="{5EEC2E2C-3288-4F5E-82D1-2929FCEC1714}"/>
   </bookViews>
   <sheets>
     <sheet name="chi_squared_test" sheetId="2" r:id="rId1"/>
@@ -372,7 +372,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -388,16 +388,15 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="1" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -414,12 +413,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Link" xfId="1" builtinId="8"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -437,7 +435,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -785,7 +783,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="de-DE"/>
+  <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2370,7 +2368,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2668,161 +2666,161 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A7A0348-C0D0-4693-8739-97C81837FDBE}">
   <dimension ref="B2:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.44140625" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.5546875" style="1"/>
+    <col min="1" max="1" width="5.453125" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="2:10" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="13" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B13" s="27" t="s">
+    <row r="13" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B13" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="G13" s="27" t="s">
+      <c r="G13" s="26" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B15" s="22"/>
-      <c r="C15" s="23">
+    <row r="15" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="B15" s="21"/>
+      <c r="C15" s="22">
         <v>0</v>
       </c>
-      <c r="D15" s="23">
+      <c r="D15" s="22">
         <v>1</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="22"/>
-      <c r="H15" s="23">
+      <c r="G15" s="21"/>
+      <c r="H15" s="22">
         <v>0</v>
       </c>
-      <c r="I15" s="23">
+      <c r="I15" s="22">
         <v>1</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="22" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B16" s="23">
+    <row r="16" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="B16" s="22">
         <v>1</v>
       </c>
-      <c r="C16" s="24">
-        <v>34</v>
-      </c>
-      <c r="D16" s="24">
-        <v>76</v>
-      </c>
-      <c r="E16" s="23">
+      <c r="C16" s="23">
+        <v>45</v>
+      </c>
+      <c r="D16" s="23">
+        <v>65</v>
+      </c>
+      <c r="E16" s="22">
         <f>SUM(C16:D16)</f>
         <v>110</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="22">
         <v>1</v>
       </c>
-      <c r="H16" s="28">
+      <c r="H16" s="27">
         <f>C18*E16/E18</f>
-        <v>62</v>
-      </c>
-      <c r="I16" s="28">
+        <v>63.088235294117645</v>
+      </c>
+      <c r="I16" s="27">
         <f>D18*E16/E18</f>
-        <v>48</v>
-      </c>
-      <c r="J16" s="23">
+        <v>46.911764705882355</v>
+      </c>
+      <c r="J16" s="22">
         <f>SUM(H16:I16)</f>
         <v>110</v>
       </c>
     </row>
-    <row r="17" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B17" s="23">
+    <row r="17" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="B17" s="22">
         <v>0</v>
       </c>
-      <c r="C17" s="24">
-        <v>152</v>
-      </c>
-      <c r="D17" s="24">
-        <v>68</v>
-      </c>
-      <c r="E17" s="23">
+      <c r="C17" s="23">
+        <v>72</v>
+      </c>
+      <c r="D17" s="23">
+        <v>22</v>
+      </c>
+      <c r="E17" s="22">
         <f>SUM(C17:D17)</f>
-        <v>220</v>
-      </c>
-      <c r="G17" s="23">
+        <v>94</v>
+      </c>
+      <c r="G17" s="22">
         <v>0</v>
       </c>
-      <c r="H17" s="28">
+      <c r="H17" s="27">
         <f>C18*E17/E18</f>
-        <v>124</v>
-      </c>
-      <c r="I17" s="28">
+        <v>53.911764705882355</v>
+      </c>
+      <c r="I17" s="27">
         <f>D18*E17/E18</f>
-        <v>96</v>
-      </c>
-      <c r="J17" s="23">
+        <v>40.088235294117645</v>
+      </c>
+      <c r="J17" s="22">
         <f>SUM(H17:I17)</f>
-        <v>220</v>
-      </c>
-    </row>
-    <row r="18" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B18" s="23" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="13" x14ac:dyDescent="0.3">
+      <c r="B18" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="C18" s="23">
+      <c r="C18" s="22">
         <f>SUM(C16:C17)</f>
-        <v>186</v>
-      </c>
-      <c r="D18" s="23">
+        <v>117</v>
+      </c>
+      <c r="D18" s="22">
         <f>SUM(D16:D17)</f>
-        <v>144</v>
-      </c>
-      <c r="E18" s="23">
+        <v>87</v>
+      </c>
+      <c r="E18" s="22">
         <f>SUM(C16:D17)</f>
-        <v>330</v>
-      </c>
-      <c r="G18" s="23" t="s">
+        <v>204</v>
+      </c>
+      <c r="G18" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="22">
         <f>SUM(H16:H17)</f>
-        <v>186</v>
-      </c>
-      <c r="I18" s="23">
+        <v>117</v>
+      </c>
+      <c r="I18" s="22">
         <f>SUM(I16:I17)</f>
-        <v>144</v>
-      </c>
-      <c r="J18" s="23">
+        <v>87</v>
+      </c>
+      <c r="J18" s="22">
         <f>SUM(H16:I17)</f>
-        <v>330</v>
-      </c>
-    </row>
-    <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B20" s="20" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B21" s="25">
+      <c r="B21" s="24">
         <f>((C16-H16)^2/H16) + ((C17-H17)^2/H17) +  ((D16-I16)^2/I16) +  ((D17-I17)^2/I17)</f>
-        <v>43.467741935483865</v>
+        <v>26.391085070468772</v>
       </c>
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B22" s="26" t="s">
+      <c r="B22" s="25" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="24" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B24" s="21" t="s">
+    <row r="24" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B24" s="20" t="s">
         <v>22</v>
       </c>
     </row>
@@ -2833,17 +2831,17 @@
       </c>
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B26" s="26" t="s">
+      <c r="B26" s="25" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B28" s="21" t="s">
+    <row r="28" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B28" s="20" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="29" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>24</v>
       </c>
     </row>
@@ -2852,7 +2850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:10" ht="15" x14ac:dyDescent="0.35">
+    <row r="32" spans="2:10" ht="14.5" x14ac:dyDescent="0.4">
       <c r="B32" s="1" t="s">
         <v>25</v>
       </c>
@@ -2874,61 +2872,49 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{284DBAAB-906E-4743-ADC0-64CD81757EA4}">
-  <dimension ref="B2:S54"/>
+  <dimension ref="B2:R54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M18" sqref="M18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" style="1" customWidth="1"/>
-    <col min="2" max="2" width="9.33203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="9.36328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="13" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.44140625" style="1"/>
-    <col min="6" max="6" width="9.33203125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.453125" style="1"/>
+    <col min="6" max="6" width="9.36328125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9" style="1" customWidth="1"/>
-    <col min="8" max="8" width="22.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="21.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="11.44140625" style="1"/>
+    <col min="8" max="8" width="22.08984375" style="1" customWidth="1"/>
+    <col min="9" max="9" width="21.36328125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="11.54296875" style="1" customWidth="1"/>
+    <col min="11" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:19" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B2" s="30" t="s">
+    <row r="2" spans="2:18" ht="17.5" x14ac:dyDescent="0.35">
+      <c r="B2" s="28" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="2:19" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" s="21"/>
-    </row>
-    <row r="4" spans="2:19" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="16"/>
-      <c r="C4" s="16"/>
-      <c r="D4" s="16" t="s">
+    <row r="3" spans="2:18" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="20"/>
+    </row>
+    <row r="4" spans="2:18" ht="17.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="15"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="16"/>
-      <c r="F4" s="16"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-    </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="O5" s="29"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="29"/>
-      <c r="R5" s="29"/>
-      <c r="S5" s="29"/>
-    </row>
-    <row r="6" spans="2:19" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+    </row>
+    <row r="6" spans="2:18" ht="15" x14ac:dyDescent="0.4">
       <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
@@ -2953,13 +2939,11 @@
       <c r="J6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="O6" s="29"/>
       <c r="P6" s="13"/>
       <c r="Q6" s="13"/>
       <c r="R6" s="13"/>
-      <c r="S6" s="29"/>
-    </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>1</v>
       </c>
@@ -2989,13 +2973,8 @@
         <f>G7^2</f>
         <v>6.25</v>
       </c>
-      <c r="O7" s="29"/>
-      <c r="P7" s="14"/>
-      <c r="Q7" s="14"/>
-      <c r="R7" s="14"/>
-      <c r="S7" s="29"/>
-    </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>2</v>
       </c>
@@ -3025,13 +3004,8 @@
         <f t="shared" ref="J8:J12" si="4">G8^2</f>
         <v>1.959999999999996</v>
       </c>
-      <c r="O8" s="29"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="14"/>
-      <c r="S8" s="29"/>
-    </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>3</v>
       </c>
@@ -3061,13 +3035,8 @@
         <f t="shared" si="4"/>
         <v>0.36000000000000171</v>
       </c>
-      <c r="O9" s="29"/>
-      <c r="P9" s="29"/>
-      <c r="Q9" s="29"/>
-      <c r="R9" s="29"/>
-      <c r="S9" s="29"/>
-    </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>4</v>
       </c>
@@ -3097,13 +3066,8 @@
         <f t="shared" si="4"/>
         <v>1.959999999999996</v>
       </c>
-      <c r="O10" s="29"/>
-      <c r="P10" s="29"/>
-      <c r="Q10" s="29"/>
-      <c r="R10" s="29"/>
-      <c r="S10" s="29"/>
-    </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>5</v>
       </c>
@@ -3133,13 +3097,8 @@
         <f t="shared" si="4"/>
         <v>0.25</v>
       </c>
-      <c r="O11" s="29"/>
-      <c r="P11" s="29"/>
-      <c r="Q11" s="29"/>
-      <c r="R11" s="29"/>
-      <c r="S11" s="29"/>
-    </row>
-    <row r="12" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>6</v>
       </c>
@@ -3169,13 +3128,8 @@
         <f t="shared" si="4"/>
         <v>12.96000000000001</v>
       </c>
-      <c r="O12" s="29"/>
-      <c r="P12" s="29"/>
-      <c r="Q12" s="29"/>
-      <c r="R12" s="29"/>
-      <c r="S12" s="29"/>
-    </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="2:18" ht="13" x14ac:dyDescent="0.3">
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
@@ -3204,7 +3158,7 @@
         <v>23.740000000000002</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:18" ht="13" x14ac:dyDescent="0.3">
       <c r="I16" s="3" t="s">
         <v>10</v>
       </c>
@@ -3213,11 +3167,11 @@
         <v>0.8983004457482282</v>
       </c>
     </row>
-    <row r="17" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I17" s="18"/>
-      <c r="J17" s="20"/>
-    </row>
-    <row r="18" spans="9:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="I17" s="17"/>
+      <c r="J17" s="19"/>
+    </row>
+    <row r="18" spans="9:12" ht="13" x14ac:dyDescent="0.3">
       <c r="I18" s="3" t="s">
         <v>14</v>
       </c>
@@ -3232,35 +3186,28 @@
       <c r="I19" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="K19" s="14"/>
-      <c r="L19" s="14"/>
-    </row>
-    <row r="20" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I20" s="18"/>
-      <c r="J20" s="19"/>
-      <c r="K20" s="14"/>
-      <c r="L20" s="14"/>
-    </row>
-    <row r="21" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="J21" s="14"/>
+    </row>
+    <row r="20" spans="9:12" ht="13" x14ac:dyDescent="0.3">
+      <c r="I20" s="17"/>
+      <c r="J20" s="18"/>
     </row>
     <row r="25" spans="9:12" x14ac:dyDescent="0.25">
-      <c r="I25" s="17"/>
-    </row>
-    <row r="33" spans="2:10" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B33" s="16"/>
-      <c r="C33" s="16"/>
-      <c r="D33" s="16" t="s">
+      <c r="I25" s="16"/>
+    </row>
+    <row r="33" spans="2:10" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B33" s="15"/>
+      <c r="C33" s="15"/>
+      <c r="D33" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="E33" s="16"/>
-      <c r="F33" s="16"/>
-      <c r="G33" s="16"/>
-      <c r="H33" s="16"/>
-      <c r="I33" s="16"/>
-      <c r="J33" s="16"/>
-    </row>
-    <row r="35" spans="2:10" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="E33" s="15"/>
+      <c r="F33" s="15"/>
+      <c r="G33" s="15"/>
+      <c r="H33" s="15"/>
+      <c r="I33" s="15"/>
+      <c r="J33" s="15"/>
+    </row>
+    <row r="35" spans="2:10" ht="15" x14ac:dyDescent="0.4">
       <c r="B35" s="3" t="s">
         <v>0</v>
       </c>
@@ -3472,7 +3419,7 @@
         <v>12.96000000000001</v>
       </c>
     </row>
-    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="B43" s="4" t="s">
         <v>7</v>
       </c>
@@ -3501,7 +3448,7 @@
         <v>23.740000000000002</v>
       </c>
     </row>
-    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="I45" s="3" t="s">
         <v>10</v>
       </c>
@@ -3510,16 +3457,16 @@
         <v>0.8983004457482282</v>
       </c>
     </row>
-    <row r="46" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="I46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="J46" s="15">
+      <c r="J46" s="14">
         <f>COUNT(B36:B41)</f>
         <v>6</v>
       </c>
     </row>
-    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="I47" s="3" t="s">
         <v>12</v>
       </c>
@@ -3528,7 +3475,7 @@
         <v>4.0889293929170769</v>
       </c>
     </row>
-    <row r="48" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:10" ht="13" x14ac:dyDescent="0.3">
       <c r="I48" s="3" t="s">
         <v>15</v>
       </c>
@@ -3536,10 +3483,7 @@
         <v>1.499E-2</v>
       </c>
     </row>
-    <row r="49" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="J49" s="14"/>
-    </row>
-    <row r="50" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="50" spans="9:10" ht="13" x14ac:dyDescent="0.3">
       <c r="I50" s="3" t="s">
         <v>14</v>
       </c>
@@ -3554,7 +3498,7 @@
       </c>
     </row>
     <row r="54" spans="9:10" x14ac:dyDescent="0.25">
-      <c r="I54" s="17"/>
+      <c r="I54" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>